<commit_message>
Moved database back to SQLite3 and have filled out SQL create, drop and populate scripts
</commit_message>
<xml_diff>
--- a/doc/Test Cases.xlsx
+++ b/doc/Test Cases.xlsx
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
   <si>
     <t>Family Name:</t>
   </si>
@@ -105,20 +105,6 @@
   </si>
   <si>
     <t>Student #:</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Test #
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(Number each test case)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -177,28 +163,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Example        1        </t>
-  </si>
-  <si>
-    <t>Invalid date for the 'Starts' field</t>
-  </si>
-  <si>
-    <t>Enter 30-02-2003 into the 'Starts' field</t>
-  </si>
-  <si>
-    <t>Date is rejected and user informed of reason. No data is saved.</t>
-  </si>
-  <si>
-    <t>F
-An error message was produced, but the invalid data was saved. This has been corrected by checking all fields before saving any data.</t>
-  </si>
-  <si>
-    <t>Add more rows (above) for each test case you design.</t>
-  </si>
-  <si>
-    <t>You must remove the example test case from the version you submit</t>
-  </si>
-  <si>
     <t>CSSE3004 Test Cases</t>
   </si>
   <si>
@@ -208,9 +172,6 @@
     <t>Mark</t>
   </si>
   <si>
-    <t>Semantically incorrect data for chosen as dates</t>
-  </si>
-  <si>
     <t>Choose a future date as the finish or enter a start date newer than the finish date</t>
   </si>
   <si>
@@ -254,6 +215,102 @@
   </si>
   <si>
     <t>P: Script does not execute, and instead simply displays as text</t>
+  </si>
+  <si>
+    <t>Semantically incorrect data for chosen dates</t>
+  </si>
+  <si>
+    <t>Enter "" into the 'Question' field</t>
+  </si>
+  <si>
+    <t>User is alerted that they cannot create a blank question.</t>
+  </si>
+  <si>
+    <t>User tried to submit a blank short answer or multi choice question</t>
+  </si>
+  <si>
+    <t>User tried create 11 answers for a multi choice question</t>
+  </si>
+  <si>
+    <t>Click 'Add Answer' on 'Show Question' page</t>
+  </si>
+  <si>
+    <t>User is unable  to click the add answer button as it has been removed</t>
+  </si>
+  <si>
+    <t>P: Once 10 answers are provided for a multi choice question, the user is unable to create any more.</t>
+  </si>
+  <si>
+    <t>User login</t>
+  </si>
+  <si>
+    <t>Enter username and password</t>
+  </si>
+  <si>
+    <t>User is logged in an the correct session is started</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Create a multi choice question</t>
+  </si>
+  <si>
+    <t>Click 'Multi Choice Questions'. Click 'Create Question'. Enter a question: "What is my name?"</t>
+  </si>
+  <si>
+    <t>Question is created</t>
+  </si>
+  <si>
+    <t>Create a multi choice question answer</t>
+  </si>
+  <si>
+    <t>Click 'Add an Answer'. Enter an answer: "Mark"</t>
+  </si>
+  <si>
+    <t>Answer is created for  that question</t>
+  </si>
+  <si>
+    <t>Click 'Short Answer Questions'. Click 'Create Question'. Enter a question: "What did you do on the holidays?"</t>
+  </si>
+  <si>
+    <t>Click 'Add a Keyword'. Enter a keyword: "Mark"</t>
+  </si>
+  <si>
+    <t>Create a short answer question keyword</t>
+  </si>
+  <si>
+    <t>Create a short answer question</t>
+  </si>
+  <si>
+    <t>Test #</t>
+  </si>
+  <si>
+    <t>Modify a question or answer</t>
+  </si>
+  <si>
+    <t>Click 'Edit'. Replace the current question or answer field</t>
+  </si>
+  <si>
+    <t>Question/answer is modified</t>
+  </si>
+  <si>
+    <t>Delete a question or answer</t>
+  </si>
+  <si>
+    <t>Click 'Remove'. Destroys the current question or answer</t>
+  </si>
+  <si>
+    <t>Question/answer is deleted</t>
+  </si>
+  <si>
+    <t>Search for questions made by a user between two datetimes</t>
+  </si>
+  <si>
+    <t>Choose a registered user. Enter two dates using the provided calendars. Click Search</t>
+  </si>
+  <si>
+    <t>Correct questions are returned</t>
   </si>
 </sst>
 </file>
@@ -403,13 +460,6 @@
       <family val="1"/>
     </font>
     <font>
-      <i/>
-      <sz val="8"/>
-      <color indexed="23"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -419,6 +469,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="24">
     <fill>
@@ -560,7 +616,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -690,6 +746,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -729,13 +811,13 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -749,20 +831,29 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="15" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1162,15 +1253,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" customWidth="1"/>
     <col min="2" max="2" width="31.140625" customWidth="1"/>
     <col min="3" max="3" width="37.5703125" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
@@ -1178,20 +1269,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25">
-      <c r="A1" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="A1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="3" spans="1:5">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1199,148 +1290,268 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="5">
         <v>41723562</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="63.75">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="3" t="s">
+    </row>
+    <row r="8" spans="1:5" ht="56.25">
+      <c r="A8" s="10">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="33.75">
+      <c r="A9" s="10">
+        <v>2</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="33.75">
+      <c r="A10" s="10">
+        <v>3</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="33.75">
+      <c r="A11" s="10">
+        <v>4</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="22.5">
+      <c r="A12" s="10">
+        <v>5</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" ht="33.75">
+      <c r="A13" s="10">
+        <v>6</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="22.5">
+      <c r="A14" s="10">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="56.25">
-      <c r="A8" s="4" t="s">
+      <c r="B14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="22.5">
+      <c r="A15" s="10">
         <v>8</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="10">
         <v>9</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="B16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="33.75">
+      <c r="A17" s="10">
         <v>10</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="B17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="10">
         <v>11</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="B18" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="22.5">
+      <c r="A19" s="10">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="56.25">
-      <c r="A9" s="7">
-        <v>1</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="33.75">
-      <c r="A10" s="7">
-        <v>2</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="33.75">
-      <c r="A11" s="7">
-        <v>3</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="33.75">
-      <c r="A12" s="7">
-        <v>4</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
+      <c r="B19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="22.5">
+      <c r="A20" s="11">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>14</v>
+      <c r="B20" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="22.5">
+      <c r="A21" s="12">
+        <v>15</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1348,8 +1559,8 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="0.62986111111111109" bottom="0.65972222222222221" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>